<commit_message>
update the inbound, finish SA
</commit_message>
<xml_diff>
--- a/Inbound Costs.xlsx
+++ b/Inbound Costs.xlsx
@@ -4,22 +4,23 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Tariff_Product"/>
     <sheet r:id="rId2" sheetId="2" name="Sheet1"/>
     <sheet r:id="rId3" sheetId="3" name="Inbound Tariff China"/>
-    <sheet r:id="rId4" sheetId="4" name="Inbound Europe"/>
-    <sheet r:id="rId5" sheetId="5" name="Inbound US"/>
-    <sheet r:id="rId6" sheetId="6" name="Inbound"/>
-    <sheet r:id="rId7" sheetId="7" name="__AIMMS_SETUP__"/>
+    <sheet r:id="rId4" sheetId="4" name="Gas Emission Inbound"/>
+    <sheet r:id="rId5" sheetId="5" name="Inbound Europe"/>
+    <sheet r:id="rId6" sheetId="6" name="Inbound US"/>
+    <sheet r:id="rId7" sheetId="7" name="Inbound"/>
+    <sheet r:id="rId8" sheetId="8" name="__AIMMS_SETUP__"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5">Inbound!$A$1:$D$41</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3">'Inbound Europe'!$A$3:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6">Inbound!$A$1:$D$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'Inbound Europe'!$A$3:$C$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">'Inbound Tariff China'!$A$3:$C$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'Inbound US'!$A$6:$B$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Inbound US'!$A$6:$B$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Tariff_Product!$A$1:$E$11</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="69">
   <si>
     <t>Initialization</t>
   </si>
@@ -131,12 +132,6 @@
     <t>tariff</t>
   </si>
   <si>
-    <t>gas_emission_chair</t>
-  </si>
-  <si>
-    <t>gas_emission_scooter</t>
-  </si>
-  <si>
     <t>ND</t>
   </si>
   <si>
@@ -173,16 +168,25 @@
     <t>factory</t>
   </si>
   <si>
-    <t>gas_emission_rope</t>
-  </si>
-  <si>
     <t>Poznan</t>
   </si>
   <si>
     <t>State</t>
   </si>
   <si>
-    <t>gas_emission_yoga_swing_blender</t>
+    <t>blender</t>
+  </si>
+  <si>
+    <t>swing</t>
+  </si>
+  <si>
+    <t>chair</t>
+  </si>
+  <si>
+    <t>scooter</t>
+  </si>
+  <si>
+    <t>skiprope</t>
   </si>
   <si>
     <t>From plant in China (yoga swing &amp; blender)</t>
@@ -225,21 +229,6 @@
   </si>
   <si>
     <t>Total_Cost_product</t>
-  </si>
-  <si>
-    <t>blender</t>
-  </si>
-  <si>
-    <t>swing</t>
-  </si>
-  <si>
-    <t>scooter</t>
-  </si>
-  <si>
-    <t>chair</t>
-  </si>
-  <si>
-    <t>skiprope</t>
   </si>
   <si>
     <t>rope</t>
@@ -294,12 +283,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -317,6 +300,12 @@
       <sz val="10"/>
       <color rgb="FFff0000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -400,6 +389,34 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
@@ -414,38 +431,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFc6c6c6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -482,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="63">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -544,110 +533,128 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -960,12 +967,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="32" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="28" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="56" width="15.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="56" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="56" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="28" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="30" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="61" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="62" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="62" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="62" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="61" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -973,65 +980,65 @@
     <col min="11" max="11" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="33" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="33" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="33" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="33" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="33" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="33" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="F1" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="J1" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="L1" s="52" t="s">
-        <v>71</v>
-      </c>
       <c r="M1" s="2"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="23">
-      <c r="A2" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="34">
+      <c r="A2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="39">
         <v>2500</v>
       </c>
-      <c r="C2" s="34">
+      <c r="C2" s="39">
         <v>2500</v>
       </c>
       <c r="D2" s="25">
@@ -1043,43 +1050,43 @@
       <c r="F2" s="25">
         <v>3500</v>
       </c>
-      <c r="G2" s="53"/>
-      <c r="H2" s="26">
+      <c r="G2" s="21"/>
+      <c r="H2" s="57">
         <v>3</v>
       </c>
-      <c r="I2" s="26">
+      <c r="I2" s="57">
         <v>1</v>
       </c>
-      <c r="J2" s="26">
+      <c r="J2" s="57">
         <v>6</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="57">
         <v>3</v>
       </c>
-      <c r="L2" s="26">
+      <c r="L2" s="57">
         <v>7</v>
       </c>
-      <c r="M2" s="53"/>
-      <c r="N2" s="26">
+      <c r="M2" s="21"/>
+      <c r="N2" s="57">
         <f>B2*H2</f>
       </c>
-      <c r="O2" s="26">
+      <c r="O2" s="57">
         <f>C2*I2</f>
       </c>
-      <c r="P2" s="26">
+      <c r="P2" s="57">
         <f>D2*J2</f>
       </c>
-      <c r="Q2" s="26">
+      <c r="Q2" s="57">
         <f>E2*K2</f>
       </c>
-      <c r="R2" s="26">
+      <c r="R2" s="57">
         <f>F2*L2</f>
       </c>
-      <c r="S2" s="30"/>
+      <c r="S2" s="58"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="23">
       <c r="A3" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="25">
         <v>2500</v>
@@ -1096,43 +1103,43 @@
       <c r="F3" s="25">
         <v>2900</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="26">
+      <c r="G3" s="21"/>
+      <c r="H3" s="57">
         <v>21</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="57">
         <v>1</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="57">
         <v>1</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="57">
         <v>19</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="57">
         <v>59</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="26">
+      <c r="M3" s="21"/>
+      <c r="N3" s="57">
         <f>B3*H3</f>
       </c>
-      <c r="O3" s="26">
+      <c r="O3" s="57">
         <f>C3*I3</f>
       </c>
-      <c r="P3" s="26">
+      <c r="P3" s="57">
         <f>D3*J3</f>
       </c>
-      <c r="Q3" s="26">
+      <c r="Q3" s="57">
         <f>E3*K3</f>
       </c>
-      <c r="R3" s="26">
+      <c r="R3" s="57">
         <f>F3*L3</f>
       </c>
-      <c r="S3" s="30"/>
+      <c r="S3" s="58"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="23">
       <c r="A4" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="25">
         <v>3000</v>
@@ -1149,43 +1156,43 @@
       <c r="F4" s="25">
         <v>3000</v>
       </c>
-      <c r="G4" s="53"/>
-      <c r="H4" s="26">
+      <c r="G4" s="21"/>
+      <c r="H4" s="57">
         <v>15</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="57">
         <v>1</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="57">
         <v>1</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="57">
         <v>14</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="57">
         <v>41</v>
       </c>
-      <c r="M4" s="53"/>
-      <c r="N4" s="26">
+      <c r="M4" s="21"/>
+      <c r="N4" s="57">
         <f>B4*H4</f>
       </c>
-      <c r="O4" s="26">
+      <c r="O4" s="57">
         <f>C4*I4</f>
       </c>
-      <c r="P4" s="26">
+      <c r="P4" s="57">
         <f>D4*J4</f>
       </c>
-      <c r="Q4" s="26">
+      <c r="Q4" s="57">
         <f>E4*K4</f>
       </c>
-      <c r="R4" s="26">
+      <c r="R4" s="57">
         <f>F4*L4</f>
       </c>
-      <c r="S4" s="30"/>
+      <c r="S4" s="58"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="23">
       <c r="A5" s="24" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B5" s="25">
         <v>2750</v>
@@ -1202,33 +1209,33 @@
       <c r="F5" s="25">
         <v>2500</v>
       </c>
-      <c r="G5" s="53"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="26">
+      <c r="G5" s="21"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="57">
         <f>B5*H5</f>
       </c>
-      <c r="O5" s="26">
+      <c r="O5" s="57">
         <f>C5*I5</f>
       </c>
-      <c r="P5" s="26">
+      <c r="P5" s="57">
         <f>D5*J5</f>
       </c>
-      <c r="Q5" s="26">
+      <c r="Q5" s="57">
         <f>E5*K5</f>
       </c>
-      <c r="R5" s="26">
+      <c r="R5" s="57">
         <f>F5*L5</f>
       </c>
-      <c r="S5" s="30"/>
+      <c r="S5" s="58"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="23">
       <c r="A6" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="25">
         <v>3500</v>
@@ -1245,43 +1252,43 @@
       <c r="F6" s="25">
         <v>2400</v>
       </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="26">
+      <c r="G6" s="21"/>
+      <c r="H6" s="57">
         <v>17</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="57">
         <v>1</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="57">
         <v>1</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="57">
         <v>15</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="57">
         <v>47</v>
       </c>
-      <c r="M6" s="53"/>
-      <c r="N6" s="26">
+      <c r="M6" s="21"/>
+      <c r="N6" s="57">
         <f>B6*H6</f>
       </c>
-      <c r="O6" s="26">
+      <c r="O6" s="57">
         <f>C6*I6</f>
       </c>
-      <c r="P6" s="26">
+      <c r="P6" s="57">
         <f>D6*J6</f>
       </c>
-      <c r="Q6" s="26">
+      <c r="Q6" s="57">
         <f>E6*K6</f>
       </c>
-      <c r="R6" s="26">
+      <c r="R6" s="57">
         <f>F6*L6</f>
       </c>
-      <c r="S6" s="30"/>
+      <c r="S6" s="58"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="23">
       <c r="A7" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="25">
         <v>4000</v>
@@ -1298,43 +1305,43 @@
       <c r="F7" s="25">
         <v>1000</v>
       </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="26">
+      <c r="G7" s="21"/>
+      <c r="H7" s="57">
         <v>17</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="57">
         <v>1</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="57">
         <v>1</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="57">
         <v>16</v>
       </c>
-      <c r="L7" s="26">
+      <c r="L7" s="57">
         <v>49</v>
       </c>
-      <c r="M7" s="53"/>
-      <c r="N7" s="26">
+      <c r="M7" s="21"/>
+      <c r="N7" s="57">
         <f>B7*H7</f>
       </c>
-      <c r="O7" s="26">
+      <c r="O7" s="57">
         <f>C7*I7</f>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="57">
         <f>D7*J7</f>
       </c>
-      <c r="Q7" s="26">
+      <c r="Q7" s="57">
         <f>E7*K7</f>
       </c>
-      <c r="R7" s="26">
+      <c r="R7" s="57">
         <f>F7*L7</f>
       </c>
-      <c r="S7" s="30"/>
+      <c r="S7" s="58"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="23">
       <c r="A8" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="25">
         <v>3450</v>
@@ -1342,7 +1349,7 @@
       <c r="C8" s="25">
         <v>3450</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="26">
         <v>1350</v>
       </c>
       <c r="E8" s="25">
@@ -1351,33 +1358,33 @@
       <c r="F8" s="25">
         <v>2650</v>
       </c>
-      <c r="G8" s="53"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="26">
+      <c r="G8" s="21"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="57">
         <f>B8*H8</f>
       </c>
-      <c r="O8" s="26">
+      <c r="O8" s="57">
         <f>C8*I8</f>
       </c>
-      <c r="P8" s="26">
+      <c r="P8" s="57">
         <f>D8*J8</f>
       </c>
-      <c r="Q8" s="26">
+      <c r="Q8" s="57">
         <f>E8*K8</f>
       </c>
-      <c r="R8" s="26">
+      <c r="R8" s="57">
         <f>F8*L8</f>
       </c>
-      <c r="S8" s="30"/>
+      <c r="S8" s="58"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="25">
         <v>3000</v>
@@ -1395,42 +1402,42 @@
         <v>2000</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="54">
+      <c r="H9" s="3">
         <v>14</v>
       </c>
-      <c r="I9" s="54">
+      <c r="I9" s="3">
         <v>1</v>
       </c>
-      <c r="J9" s="54">
+      <c r="J9" s="3">
         <v>1</v>
       </c>
-      <c r="K9" s="54">
+      <c r="K9" s="3">
         <v>13</v>
       </c>
-      <c r="L9" s="54">
+      <c r="L9" s="3">
         <v>39</v>
       </c>
       <c r="M9" s="2"/>
-      <c r="N9" s="26">
+      <c r="N9" s="57">
         <f>B9*H9</f>
       </c>
-      <c r="O9" s="26">
+      <c r="O9" s="57">
         <f>C9*I9</f>
       </c>
-      <c r="P9" s="26">
+      <c r="P9" s="57">
         <f>D9*J9</f>
       </c>
-      <c r="Q9" s="26">
+      <c r="Q9" s="57">
         <f>E9*K9</f>
       </c>
-      <c r="R9" s="26">
+      <c r="R9" s="57">
         <f>F9*L9</f>
       </c>
-      <c r="S9" s="55"/>
+      <c r="S9" s="59"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="23">
       <c r="A10" s="24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="25">
         <v>3500</v>
@@ -1441,39 +1448,39 @@
       <c r="D10" s="25">
         <v>6000</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="26">
         <v>1350</v>
       </c>
       <c r="F10" s="25">
         <v>3500</v>
       </c>
-      <c r="G10" s="53"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="26">
+      <c r="G10" s="21"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="57">
         <f>B10*H10</f>
       </c>
-      <c r="O10" s="26">
+      <c r="O10" s="57">
         <f>C10*I10</f>
       </c>
-      <c r="P10" s="26">
+      <c r="P10" s="57">
         <f>D10*J10</f>
       </c>
-      <c r="Q10" s="26">
+      <c r="Q10" s="57">
         <f>E10*K10</f>
       </c>
-      <c r="R10" s="26">
+      <c r="R10" s="57">
         <f>F10*L10</f>
       </c>
-      <c r="S10" s="30"/>
+      <c r="S10" s="58"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="25">
         <v>2500</v>
@@ -1481,56 +1488,56 @@
       <c r="C11" s="25">
         <v>2500</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="26">
         <v>3150</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="26">
         <v>500</v>
       </c>
       <c r="F11" s="25">
         <v>3500</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="54">
+      <c r="H11" s="3">
         <v>4</v>
       </c>
-      <c r="I11" s="54">
+      <c r="I11" s="3">
         <v>1</v>
       </c>
-      <c r="J11" s="54">
+      <c r="J11" s="3">
         <v>1</v>
       </c>
-      <c r="K11" s="54">
+      <c r="K11" s="3">
         <v>4</v>
       </c>
-      <c r="L11" s="54">
+      <c r="L11" s="3">
         <v>12</v>
       </c>
       <c r="M11" s="2"/>
-      <c r="N11" s="26">
+      <c r="N11" s="57">
         <f>B11*H11</f>
       </c>
-      <c r="O11" s="26">
+      <c r="O11" s="57">
         <f>C11*I11</f>
       </c>
-      <c r="P11" s="26">
+      <c r="P11" s="57">
         <f>D11*J11</f>
       </c>
-      <c r="Q11" s="26">
+      <c r="Q11" s="57">
         <f>E11*K11</f>
       </c>
-      <c r="R11" s="26">
+      <c r="R11" s="57">
         <f>F11*L11</f>
       </c>
-      <c r="S11" s="30"/>
+      <c r="S11" s="56"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="22"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="21"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="60"/>
       <c r="G12" s="2"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1538,22 +1545,22 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="26">
+      <c r="N12" s="57">
         <f>SUM(N2:N11)</f>
       </c>
-      <c r="O12" s="26">
+      <c r="O12" s="57">
         <f>SUM(O2:O11)</f>
       </c>
-      <c r="P12" s="26">
+      <c r="P12" s="57">
         <f>SUM(P2:P11)</f>
       </c>
-      <c r="Q12" s="26">
+      <c r="Q12" s="57">
         <f>SUM(Q2:Q11)</f>
       </c>
-      <c r="R12" s="26">
+      <c r="R12" s="57">
         <f>SUM(R2:R11)</f>
       </c>
-      <c r="S12" s="26">
+      <c r="S12" s="57">
         <f>SUM(N12:R12)</f>
       </c>
     </row>
@@ -1573,13 +1580,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="32" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="30" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="32" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="30" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -1589,290 +1596,290 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="36"/>
-      <c r="B1" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="38" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="C1" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="E1" s="43" t="s">
         <v>57</v>
       </c>
+      <c r="F1" s="44" t="s">
+        <v>58</v>
+      </c>
       <c r="G1" s="22"/>
-      <c r="H1" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="38" t="s">
+      <c r="H1" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="I1" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="J1" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="K1" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="40"/>
+      <c r="L1" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="45"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="36"/>
-      <c r="B2" s="41">
+      <c r="A2" s="41"/>
+      <c r="B2" s="46">
         <v>3</v>
       </c>
-      <c r="C2" s="42">
+      <c r="C2" s="47">
         <v>3</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="47">
         <v>6</v>
       </c>
-      <c r="E2" s="42">
+      <c r="E2" s="47">
         <v>7</v>
       </c>
-      <c r="F2" s="43">
+      <c r="F2" s="48">
         <v>1</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="41">
+      <c r="G2" s="28"/>
+      <c r="H2" s="46">
         <f>Tariff_Product!C2*B2</f>
       </c>
-      <c r="I2" s="42">
+      <c r="I2" s="47">
         <f>Tariff_Product!C2*F2</f>
       </c>
-      <c r="J2" s="42">
+      <c r="J2" s="47">
         <f>Tariff_Product!D2*D2</f>
       </c>
-      <c r="K2" s="42">
+      <c r="K2" s="47">
         <f>Tariff_Product!E2*C2</f>
       </c>
-      <c r="L2" s="42">
+      <c r="L2" s="47">
         <f>Tariff_Product!F2*E2</f>
       </c>
       <c r="M2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="36"/>
-      <c r="B3" s="41">
+      <c r="A3" s="41"/>
+      <c r="B3" s="46">
         <v>21</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="47">
         <v>19</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="47">
         <v>1</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="47">
         <v>59</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="48">
         <v>1</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="41">
+      <c r="G3" s="28"/>
+      <c r="H3" s="46">
         <f>Tariff_Product!C3*B3</f>
       </c>
-      <c r="I3" s="42">
+      <c r="I3" s="47">
         <f>Tariff_Product!C3*F3</f>
       </c>
-      <c r="J3" s="42">
+      <c r="J3" s="47">
         <f>Tariff_Product!D3*D3</f>
       </c>
-      <c r="K3" s="42">
+      <c r="K3" s="47">
         <f>Tariff_Product!E3*C3</f>
       </c>
-      <c r="L3" s="42">
+      <c r="L3" s="47">
         <f>Tariff_Product!F3*E3</f>
       </c>
       <c r="M3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="36"/>
-      <c r="B4" s="41">
+      <c r="A4" s="41"/>
+      <c r="B4" s="46">
         <v>15</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="47">
         <v>14</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="47">
         <v>1</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="47">
         <v>41</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="48">
         <v>1</v>
       </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="41">
+      <c r="G4" s="28"/>
+      <c r="H4" s="46">
         <f>Tariff_Product!C4*B4</f>
       </c>
-      <c r="I4" s="42">
+      <c r="I4" s="47">
         <f>Tariff_Product!C4*F4</f>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="47">
         <f>Tariff_Product!D4*D4</f>
       </c>
-      <c r="K4" s="42">
+      <c r="K4" s="47">
         <f>Tariff_Product!E4*C4</f>
       </c>
-      <c r="L4" s="42">
+      <c r="L4" s="47">
         <f>Tariff_Product!F4*E4</f>
       </c>
       <c r="M4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="36"/>
-      <c r="B5" s="41">
+      <c r="A5" s="41"/>
+      <c r="B5" s="46">
         <v>17</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="47">
         <v>15</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="47">
         <v>1</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="47">
         <v>47</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="48">
         <v>1</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="41">
+      <c r="G5" s="28"/>
+      <c r="H5" s="46">
         <f>Tariff_Product!C5*B5</f>
       </c>
-      <c r="I5" s="42">
+      <c r="I5" s="47">
         <f>Tariff_Product!C5*F5</f>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="47">
         <f>Tariff_Product!D5*D5</f>
       </c>
-      <c r="K5" s="42">
+      <c r="K5" s="47">
         <f>Tariff_Product!E5*C5</f>
       </c>
-      <c r="L5" s="42">
+      <c r="L5" s="47">
         <f>Tariff_Product!F5*E5</f>
       </c>
       <c r="M5" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="36"/>
-      <c r="B6" s="41">
+      <c r="A6" s="41"/>
+      <c r="B6" s="46">
         <v>17</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="47">
         <v>16</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="47">
         <v>1</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="47">
         <v>49</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="48">
         <v>1</v>
       </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="41">
+      <c r="G6" s="28"/>
+      <c r="H6" s="46">
         <f>Tariff_Product!C6*B6</f>
       </c>
-      <c r="I6" s="42">
+      <c r="I6" s="47">
         <f>Tariff_Product!C6*F6</f>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="47">
         <f>Tariff_Product!D6*D6</f>
       </c>
-      <c r="K6" s="42">
+      <c r="K6" s="47">
         <f>Tariff_Product!E6*C6</f>
       </c>
-      <c r="L6" s="42">
+      <c r="L6" s="47">
         <f>Tariff_Product!F6*E6</f>
       </c>
       <c r="M6" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="36"/>
-      <c r="B7" s="41">
+      <c r="A7" s="41"/>
+      <c r="B7" s="46">
         <v>14</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="47">
         <v>13</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="47">
         <v>1</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="47">
         <v>39</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="48">
         <v>1</v>
       </c>
-      <c r="G7" s="29"/>
-      <c r="H7" s="41">
+      <c r="G7" s="28"/>
+      <c r="H7" s="46">
         <f>Tariff_Product!C7*B7</f>
       </c>
-      <c r="I7" s="42">
+      <c r="I7" s="47">
         <f>Tariff_Product!C7*F7</f>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="47">
         <f>Tariff_Product!D7*D7</f>
       </c>
-      <c r="K7" s="42">
+      <c r="K7" s="47">
         <f>Tariff_Product!E7*C7</f>
       </c>
-      <c r="L7" s="42">
+      <c r="L7" s="47">
         <f>Tariff_Product!F7*E7</f>
       </c>
       <c r="M7" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="36"/>
-      <c r="B8" s="41">
+      <c r="A8" s="41"/>
+      <c r="B8" s="46">
         <v>4</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="47">
         <v>4</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="47">
         <v>1</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="47">
         <v>12</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="48">
         <v>1</v>
       </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="44">
+      <c r="G8" s="28"/>
+      <c r="H8" s="49">
         <f>Tariff_Product!C8*B8</f>
       </c>
-      <c r="I8" s="45">
+      <c r="I8" s="50">
         <f>Tariff_Product!C8*F8</f>
       </c>
-      <c r="J8" s="45">
+      <c r="J8" s="50">
         <f>Tariff_Product!D8*D8</f>
       </c>
-      <c r="K8" s="45">
+      <c r="K8" s="50">
         <f>Tariff_Product!E8*C8</f>
       </c>
-      <c r="L8" s="45">
+      <c r="L8" s="50">
         <f>Tariff_Product!F8*E8</f>
       </c>
-      <c r="M8" s="46" t="s">
-        <v>63</v>
+      <c r="M8" s="51" t="s">
+        <v>64</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="47" t="s">
-        <v>64</v>
+      <c r="A9" s="52" t="s">
+        <v>65</v>
       </c>
       <c r="B9" s="3">
         <f>SUM(B1:B7)</f>
@@ -1889,25 +1896,25 @@
       <c r="F9" s="3">
         <f>SUM(F1:F7)</f>
       </c>
-      <c r="G9" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="42">
+      <c r="G9" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="47">
         <f>SUM(H2:H8)</f>
       </c>
-      <c r="I9" s="42">
+      <c r="I9" s="47">
         <f>SUM(I2:I8)</f>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="47">
         <f>SUM(J2:J8)</f>
       </c>
-      <c r="K9" s="42">
+      <c r="K9" s="47">
         <f>SUM(K2:K8)</f>
       </c>
-      <c r="L9" s="42">
+      <c r="L9" s="47">
         <f>SUM(L2:L8)</f>
       </c>
-      <c r="M9" s="49">
+      <c r="M9" s="54">
         <f>SUM(H9:L9)</f>
       </c>
     </row>
@@ -1921,16 +1928,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="32" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="32" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="30" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="30" width="19.005" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="28" width="30.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1939,40 +1945,32 @@
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="4"/>
-      <c r="D1" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="12.75" customFormat="1" s="23">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="34">
+      <c r="B4" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="39">
         <v>2500</v>
-      </c>
-      <c r="D4" s="26">
-        <v>4600</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="12.75" customFormat="1" s="23">
@@ -1980,13 +1978,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="25">
         <v>2500</v>
-      </c>
-      <c r="D5" s="26">
-        <v>3400</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="12.75" customFormat="1" s="23">
@@ -1994,13 +1989,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="25">
         <v>3000</v>
-      </c>
-      <c r="D6" s="26">
-        <v>3100</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="12.75" customFormat="1" s="23">
@@ -2008,13 +2000,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="25">
         <v>2750</v>
-      </c>
-      <c r="D7" s="26">
-        <v>3400</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="12.75" customFormat="1" s="23">
@@ -2022,13 +2011,10 @@
         <v>20</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="25">
         <v>3500</v>
-      </c>
-      <c r="D8" s="26">
-        <v>3200</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="12.75" customFormat="1" s="23">
@@ -2036,13 +2022,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="25">
         <v>4000</v>
-      </c>
-      <c r="D9" s="26">
-        <v>3300</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="12.75" customFormat="1" s="23">
@@ -2050,13 +2033,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="25">
         <v>3450</v>
-      </c>
-      <c r="D10" s="26">
-        <v>3500</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="12.75" customFormat="1" s="23">
@@ -2064,13 +2044,10 @@
         <v>22</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="25">
         <v>3000</v>
-      </c>
-      <c r="D11" s="26">
-        <v>4600</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="12.75" customFormat="1" s="23">
@@ -2078,13 +2055,10 @@
         <v>19</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" s="25">
         <v>3500</v>
-      </c>
-      <c r="D12" s="26">
-        <v>3200</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="12.75" customFormat="1" s="23">
@@ -2092,28 +2066,23 @@
         <v>23</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="25">
         <v>2500</v>
       </c>
-      <c r="D13" s="26">
-        <v>1900</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="35"/>
+      <c r="A15" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="40"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2125,183 +2094,237 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="32" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="32" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="16.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="33" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="37" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="30"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="30"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="32.25">
+      <c r="A1" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="12.75" customFormat="1" s="23">
-      <c r="A4" s="24" t="s">
+      <c r="C1" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="D1" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="23">
+      <c r="A2" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="35">
+        <v>4600</v>
+      </c>
+      <c r="C2" s="35">
+        <v>4600</v>
+      </c>
+      <c r="D2" s="35">
+        <v>180</v>
+      </c>
+      <c r="E2" s="35">
+        <v>250</v>
+      </c>
+      <c r="F2" s="35">
+        <v>1200</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="23">
+      <c r="A3" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="35">
+        <v>3400</v>
+      </c>
+      <c r="C3" s="35">
+        <v>3400</v>
+      </c>
+      <c r="D3" s="35">
+        <v>250</v>
+      </c>
+      <c r="E3" s="35">
+        <v>150</v>
+      </c>
+      <c r="F3" s="35">
+        <v>1200</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="23">
+      <c r="A4" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="25">
+      <c r="B4" s="35">
+        <v>3100</v>
+      </c>
+      <c r="C4" s="35">
+        <v>3100</v>
+      </c>
+      <c r="D4" s="35">
+        <v>400</v>
+      </c>
+      <c r="E4" s="35">
+        <v>200</v>
+      </c>
+      <c r="F4" s="35">
+        <v>1500</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="23">
+      <c r="A5" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="35">
+        <v>3400</v>
+      </c>
+      <c r="C5" s="35">
+        <v>3400</v>
+      </c>
+      <c r="D5" s="35">
+        <v>500</v>
+      </c>
+      <c r="E5" s="35">
+        <v>280</v>
+      </c>
+      <c r="F5" s="35">
+        <v>1300</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="23">
+      <c r="A6" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="35">
+        <v>3200</v>
+      </c>
+      <c r="C6" s="35">
+        <v>3200</v>
+      </c>
+      <c r="D6" s="35">
+        <v>450</v>
+      </c>
+      <c r="E6" s="35">
+        <v>200</v>
+      </c>
+      <c r="F6" s="35">
+        <v>1300</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="23">
+      <c r="A7" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="35">
+        <v>3300</v>
+      </c>
+      <c r="C7" s="35">
+        <v>3300</v>
+      </c>
+      <c r="D7" s="35">
+        <v>300</v>
+      </c>
+      <c r="E7" s="35">
+        <v>120</v>
+      </c>
+      <c r="F7" s="35">
+        <v>1000</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="23">
+      <c r="A8" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="35">
         <v>3500</v>
       </c>
-      <c r="D4" s="26">
-        <v>1200</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="12.75" customFormat="1" s="23">
-      <c r="A5" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="25">
-        <v>2900</v>
-      </c>
-      <c r="D5" s="26">
-        <v>1200</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="12.75" customFormat="1" s="23">
-      <c r="A6" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="25">
-        <v>3000</v>
-      </c>
-      <c r="D6" s="26">
+      <c r="C8" s="35">
+        <v>3500</v>
+      </c>
+      <c r="D8" s="35">
+        <v>250</v>
+      </c>
+      <c r="E8" s="35">
+        <v>70</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1100</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="23">
+      <c r="A9" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="35">
+        <v>4600</v>
+      </c>
+      <c r="C9" s="35">
+        <v>4600</v>
+      </c>
+      <c r="D9" s="35">
+        <v>200</v>
+      </c>
+      <c r="E9" s="35">
+        <v>450</v>
+      </c>
+      <c r="F9" s="35">
+        <v>1400</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="23">
+      <c r="A10" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="35">
+        <v>3200</v>
+      </c>
+      <c r="C10" s="35">
+        <v>3200</v>
+      </c>
+      <c r="D10" s="35">
+        <v>100</v>
+      </c>
+      <c r="E10" s="35">
+        <v>500</v>
+      </c>
+      <c r="F10" s="35">
         <v>1500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="12.75" customFormat="1" s="23">
-      <c r="A7" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="25">
-        <v>2500</v>
-      </c>
-      <c r="D7" s="26">
-        <v>1300</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="12.75" customFormat="1" s="23">
-      <c r="A8" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="25">
-        <v>2400</v>
-      </c>
-      <c r="D8" s="26">
-        <v>1300</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="12.75" customFormat="1" s="23">
-      <c r="A9" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="25">
-        <v>1000</v>
-      </c>
-      <c r="D9" s="26">
-        <v>1000</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="12.75" customFormat="1" s="23">
-      <c r="A10" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="25">
-        <v>2650</v>
-      </c>
-      <c r="D10" s="26">
-        <v>1100</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="12.75" customFormat="1" s="23">
-      <c r="A11" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="24" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25" customFormat="1" s="23">
+      <c r="A11" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="25">
-        <v>2000</v>
-      </c>
-      <c r="D11" s="26">
-        <v>1400</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="12.75" customFormat="1" s="23">
-      <c r="A12" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="25">
-        <v>3500</v>
-      </c>
-      <c r="D12" s="26">
-        <v>1500</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="12.75" customFormat="1" s="23">
-      <c r="A13" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="25">
-        <v>3500</v>
-      </c>
-      <c r="D13" s="26">
+      <c r="B11" s="35">
+        <v>1900</v>
+      </c>
+      <c r="C11" s="35">
+        <v>1900</v>
+      </c>
+      <c r="D11" s="35">
+        <v>50</v>
+      </c>
+      <c r="E11" s="35">
+        <v>500</v>
+      </c>
+      <c r="F11" s="35">
         <v>1300</v>
       </c>
     </row>
@@ -2315,7 +2338,161 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="30" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="30" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="16.433571428571426" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="12.75" customFormat="1" s="23">
+      <c r="A4" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="25">
+        <v>3500</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="12.75" customFormat="1" s="23">
+      <c r="A5" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="25">
+        <v>2900</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="12.75" customFormat="1" s="23">
+      <c r="A6" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="25">
+        <v>3000</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="12.75" customFormat="1" s="23">
+      <c r="A7" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="25">
+        <v>2500</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="12.75" customFormat="1" s="23">
+      <c r="A8" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="25">
+        <v>2400</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="12.75" customFormat="1" s="23">
+      <c r="A9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="12.75" customFormat="1" s="23">
+      <c r="A10" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="25">
+        <v>2650</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="12.75" customFormat="1" s="23">
+      <c r="A11" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="25">
+        <v>2000</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="12.75" customFormat="1" s="23">
+      <c r="A12" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="25">
+        <v>3500</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="12.75" customFormat="1" s="23">
+      <c r="A13" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="25">
+        <v>3500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2323,10 +2500,9 @@
   <cols>
     <col min="1" max="1" style="6" width="19.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="28" width="16.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="27" width="16.433571428571426" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="28" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -2337,7 +2513,6 @@
       <c r="C1" s="21"/>
       <c r="D1" s="2"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="22"/>
@@ -2345,7 +2520,6 @@
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="22" t="s">
@@ -2357,7 +2531,6 @@
         <v>30</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="22" t="s">
@@ -2369,7 +2542,6 @@
         <v>32</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2"/>
@@ -2377,7 +2549,6 @@
       <c r="C5" s="21"/>
       <c r="D5" s="2"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="9" t="s">
@@ -2386,217 +2557,162 @@
       <c r="B6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>34</v>
-      </c>
+      <c r="C6" s="21"/>
       <c r="D6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="12.75" customFormat="1" s="23">
       <c r="A7" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="25">
         <v>1500</v>
       </c>
-      <c r="C7" s="26">
-        <v>180</v>
-      </c>
+      <c r="C7" s="21"/>
       <c r="D7" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" s="25">
         <v>3500</v>
       </c>
-      <c r="F7" s="26">
-        <v>250</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="12.75" customFormat="1" s="23">
       <c r="A8" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" s="25">
         <v>2200</v>
       </c>
-      <c r="C8" s="26">
-        <v>250</v>
-      </c>
+      <c r="C8" s="21"/>
       <c r="D8" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" s="25">
         <v>2150</v>
       </c>
-      <c r="F8" s="26">
-        <v>150</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="12.75" customFormat="1" s="23">
       <c r="A9" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" s="25">
         <v>2000</v>
       </c>
-      <c r="C9" s="26">
-        <v>400</v>
-      </c>
+      <c r="C9" s="21"/>
       <c r="D9" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9" s="25">
         <v>3000</v>
       </c>
-      <c r="F9" s="26">
-        <v>200</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="12.75" customFormat="1" s="23">
       <c r="A10" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="25">
         <v>3000</v>
       </c>
-      <c r="C10" s="26">
-        <v>500</v>
-      </c>
+      <c r="C10" s="21"/>
       <c r="D10" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E10" s="25">
         <v>2500</v>
       </c>
-      <c r="F10" s="26">
-        <v>280</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="12.75" customFormat="1" s="23">
       <c r="A11" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" s="25">
         <v>2500</v>
       </c>
-      <c r="C11" s="26">
-        <v>450</v>
-      </c>
+      <c r="C11" s="21"/>
       <c r="D11" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="25">
         <v>2750</v>
       </c>
-      <c r="F11" s="26">
-        <v>200</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="12.75" customFormat="1" s="23">
       <c r="A12" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="25">
         <v>2500</v>
       </c>
-      <c r="C12" s="26">
-        <v>300</v>
-      </c>
+      <c r="C12" s="21"/>
       <c r="D12" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" s="25">
         <v>2000</v>
       </c>
-      <c r="F12" s="26">
-        <v>120</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="12.75" customFormat="1" s="23">
       <c r="A13" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="25">
         <v>2200</v>
       </c>
-      <c r="C13" s="26">
-        <v>250</v>
-      </c>
+      <c r="C13" s="21"/>
       <c r="D13" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="27">
+        <v>40</v>
+      </c>
+      <c r="E13" s="26">
         <v>1350</v>
-      </c>
-      <c r="F13" s="26">
-        <v>70</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="12.75" customFormat="1" s="23">
       <c r="A14" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" s="25">
         <v>2000</v>
       </c>
-      <c r="C14" s="26">
-        <v>200</v>
-      </c>
+      <c r="C14" s="21"/>
       <c r="D14" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E14" s="25">
         <v>5000</v>
       </c>
-      <c r="F14" s="26">
-        <v>450</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="12.75" customFormat="1" s="23">
       <c r="A15" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="27">
+        <v>42</v>
+      </c>
+      <c r="B15" s="26">
         <v>1350</v>
       </c>
-      <c r="C15" s="26">
-        <v>100</v>
-      </c>
+      <c r="C15" s="21"/>
       <c r="D15" s="24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E15" s="25">
         <v>6000</v>
       </c>
-      <c r="F15" s="26">
-        <v>500</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="12.75" customFormat="1" s="23">
       <c r="A16" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="27">
+        <v>43</v>
+      </c>
+      <c r="B16" s="26">
         <v>500</v>
       </c>
-      <c r="C16" s="26">
-        <v>50</v>
-      </c>
+      <c r="C16" s="21"/>
       <c r="D16" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="27">
+        <v>43</v>
+      </c>
+      <c r="E16" s="26">
         <v>3150</v>
-      </c>
-      <c r="F16" s="26">
-        <v>500</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="12.75">
@@ -2605,7 +2721,6 @@
       <c r="C17" s="21"/>
       <c r="D17" s="2"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="12.75">
       <c r="A18" s="2"/>
@@ -2613,7 +2728,6 @@
       <c r="C18" s="21"/>
       <c r="D18" s="2"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="12.75">
       <c r="A19" s="2"/>
@@ -2621,7 +2735,6 @@
       <c r="C19" s="21"/>
       <c r="D19" s="2"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="12.75">
       <c r="A20" s="2"/>
@@ -2629,7 +2742,6 @@
       <c r="C20" s="21"/>
       <c r="D20" s="2"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="12.75">
       <c r="A21" s="2"/>
@@ -2637,7 +2749,6 @@
       <c r="C21" s="21"/>
       <c r="D21" s="2"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="12.75">
       <c r="A22" s="2"/>
@@ -2645,7 +2756,6 @@
       <c r="C22" s="21"/>
       <c r="D22" s="2"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="12.75">
       <c r="A23" s="2"/>
@@ -2653,7 +2763,6 @@
       <c r="C23" s="21"/>
       <c r="D23" s="2"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="12.75">
       <c r="A24" s="2"/>
@@ -2661,7 +2770,6 @@
       <c r="C24" s="21"/>
       <c r="D24" s="2"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="12.75">
       <c r="A25" s="2"/>
@@ -2669,7 +2777,6 @@
       <c r="C25" s="21"/>
       <c r="D25" s="2"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="21"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="12.75">
       <c r="A26" s="2"/>
@@ -2677,14 +2784,13 @@
       <c r="C26" s="21"/>
       <c r="D26" s="2"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -3750,7 +3856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>

</xml_diff>